<commit_message>
Ended with parsers. UTaK wait for additional keys
</commit_message>
<xml_diff>
--- a/backend/database.xlsx
+++ b/backend/database.xlsx
@@ -951,7 +951,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB7"/>
+  <dimension ref="A1:W7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1057,45 +1057,20 @@
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>4096 байт на сектор; рабочая нагрузка - 55 ТБ в год, 2400 часов в год (круглосуточно);</t>
+          <t>Скорость произвольного чтения (4KB) (IOPS)</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>147 мм</t>
+          <t>Скорость произвольной записи (4KB) (IOPS)</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>20.2 мм</t>
+          <t>Поддержка NVMe</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>415 грамм</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>0.56 кг</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>Скорость произвольного чтения (4KB) (IOPS)</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
-        <is>
-          <t>Скорость произвольной записи (4KB) (IOPS)</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="inlineStr">
-        <is>
-          <t>Поддержка NVMe</t>
-        </is>
-      </c>
-      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>Максимальное количество циклов перезаписи в день (DWPD)</t>
         </is>
@@ -1306,31 +1281,6 @@
           <t>28 дБ</t>
         </is>
       </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>Длина устройства</t>
-        </is>
-      </c>
-      <c r="U4" t="inlineStr">
-        <is>
-          <t>Толщина</t>
-        </is>
-      </c>
-      <c r="V4" t="inlineStr">
-        <is>
-          <t>Вес устройства</t>
-        </is>
-      </c>
-      <c r="W4" t="inlineStr">
-        <is>
-          <t>Вес упаковки (ед)</t>
-        </is>
-      </c>
-      <c r="X4" t="inlineStr">
-        <is>
-          <t>Гарантия</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1460,12 +1410,12 @@
           <t>0.5 Вт</t>
         </is>
       </c>
-      <c r="Y6" t="inlineStr">
+      <c r="T6" t="inlineStr">
         <is>
           <t>50000</t>
         </is>
       </c>
-      <c r="Z6" t="inlineStr">
+      <c r="U6" t="inlineStr">
         <is>
           <t>73000</t>
         </is>
@@ -1522,22 +1472,22 @@
           <t>3.4 Вт</t>
         </is>
       </c>
-      <c r="Y7" t="inlineStr">
+      <c r="T7" t="inlineStr">
         <is>
           <t>330000</t>
         </is>
       </c>
-      <c r="Z7" t="inlineStr">
+      <c r="U7" t="inlineStr">
         <is>
           <t>250000</t>
         </is>
       </c>
-      <c r="AA7" t="inlineStr">
+      <c r="V7" t="inlineStr">
         <is>
           <t>есть</t>
         </is>
       </c>
-      <c r="AB7" t="inlineStr">
+      <c r="W7" t="inlineStr">
         <is>
           <t>0.9</t>
         </is>
@@ -2835,7 +2785,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R6"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2904,36 +2854,6 @@
           <t>Латентность</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>512x8</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>двустороннее</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>нет</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>Ret</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>0.004 кг</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -3222,36 +3142,6 @@
       <c r="L6" t="inlineStr">
         <is>
           <t>CL11</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>Количество чипов</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>Крепление чипов</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>Радиатор охлаждения</t>
-        </is>
-      </c>
-      <c r="P6" t="inlineStr">
-        <is>
-          <t>Тип поставки</t>
-        </is>
-      </c>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t>Вес упаковки (ед)</t>
-        </is>
-      </c>
-      <c r="R6" t="inlineStr">
-        <is>
-          <t>Гарантия</t>
         </is>
       </c>
     </row>
@@ -3266,7 +3156,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AX6"/>
+  <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3292,237 +3182,67 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Intel H510</t>
+          <t>Чипсет</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>DIMM</t>
+          <t>Тип поддерживаемой памяти</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>3200 МГц</t>
+          <t>Частотная спецификация памяти</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>3200/ 3000 / 2933 / 2800 / 2666 / 2400 / 2133 МГц</t>
+          <t>Слотов памяти DDR4</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>совместимость уточняйте на сайте производителя</t>
+          <t>Максимальный объем оперативной памяти</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>Режим работы оперативной памяти</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>64 ГБ</t>
+          <t>Разъемов SATA3</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>двухканальный</t>
+          <t>Разъемов M.2</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>Кол-во внешних USB 3.0</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>Звук</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>1 шт. (клавиатура или мышь)</t>
+          <t>Форм-фактор</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Gigabit Ethernet</t>
+          <t>Питание материнской платы и процессора</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>Intel i219V</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>8 каналов (7.1)</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>Realtek ALC897</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>mATX</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>24+8 pin</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>Ret</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>0.26x0.26x0.06 м</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>0.835 кг</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>Intel H470</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>2933 МГц</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
-        <is>
-          <t>2933/2666/2400/2133 МГц</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="inlineStr">
-        <is>
-          <t>есть</t>
-        </is>
-      </c>
-      <c r="AB1" s="1" t="inlineStr">
-        <is>
-          <t>2 шт. (клавиатура и мышь)</t>
-        </is>
-      </c>
-      <c r="AC1" s="1" t="inlineStr">
-        <is>
-          <t>Realtek</t>
-        </is>
-      </c>
-      <c r="AD1" s="1" t="inlineStr">
-        <is>
-          <t>0.778 кг</t>
-        </is>
-      </c>
-      <c r="AE1" s="1" t="inlineStr">
-        <is>
-          <t>AMD B450</t>
-        </is>
-      </c>
-      <c r="AF1" s="1" t="inlineStr">
-        <is>
-          <t>3600(O.C.)/ 3466(O.C.)/ 2933/ 2667/ 2400/ 2133 МГц</t>
-        </is>
-      </c>
-      <c r="AG1" s="1" t="inlineStr">
-        <is>
-          <t>32 ГБ</t>
-        </is>
-      </c>
-      <c r="AH1" s="1" t="inlineStr">
-        <is>
-          <t>Realtek ALC887</t>
-        </is>
-      </c>
-      <c r="AI1" s="1" t="inlineStr">
-        <is>
-          <t>0.27x0.24x0.05 м</t>
-        </is>
-      </c>
-      <c r="AJ1" s="1" t="inlineStr">
-        <is>
-          <t>0.9 кг</t>
-        </is>
-      </c>
-      <c r="AK1" s="1" t="inlineStr">
-        <is>
-          <t>AMD X670</t>
-        </is>
-      </c>
-      <c r="AL1" s="1" t="inlineStr">
-        <is>
-          <t>CrossFire</t>
-        </is>
-      </c>
-      <c r="AM1" s="1" t="inlineStr">
-        <is>
-          <t>5200 МГц</t>
-        </is>
-      </c>
-      <c r="AN1" s="1" t="inlineStr">
-        <is>
-          <t>6400(OC) / 6200(OC) / 6000(OC) / 5600(OC) / 5200 / 4800 / 4400 МГц</t>
-        </is>
-      </c>
-      <c r="AO1" s="1" t="inlineStr">
-        <is>
-          <t>128 ГБ</t>
-        </is>
-      </c>
-      <c r="AP1" s="1" t="inlineStr">
-        <is>
-          <t>x16 в одноканальном, x16 + x4 в двухканальном и еще один x2</t>
-        </is>
-      </c>
-      <c r="AQ1" s="1" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="AR1" s="1" t="inlineStr">
-        <is>
-          <t>видеовыходы задействуются после установки процессора со встроенным графическим ядром</t>
-        </is>
-      </c>
-      <c r="AS1" s="1" t="inlineStr">
-        <is>
-          <t>2.5Gigabit</t>
-        </is>
-      </c>
-      <c r="AT1" s="1" t="inlineStr">
-        <is>
-          <t>ATX</t>
-        </is>
-      </c>
-      <c r="AU1" s="1" t="inlineStr">
-        <is>
-          <t>24+8+8 pin</t>
-        </is>
-      </c>
-      <c r="AV1" s="1" t="inlineStr">
-        <is>
-          <t>2.456 кг</t>
-        </is>
-      </c>
-      <c r="AW1" s="1" t="inlineStr">
-        <is>
-          <t>6666(OC) / 6600(OC) / 6400(OC) / 6200(OC) / 6000(OC) / 5600(OC) / 5200 / 4800 / 4400 МГц</t>
-        </is>
-      </c>
-      <c r="AX1" s="1" t="inlineStr">
-        <is>
-          <t>2.682 кг</t>
+          <t>Слотов памяти DDR5</t>
         </is>
       </c>
     </row>
@@ -3544,102 +3264,62 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Тип поддерживаемой памяти</t>
+          <t>Intel H510</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Частотная спецификация памяти</t>
+          <t>DIMM</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Поддержка частот оперативной памяти</t>
+          <t>3200 МГц</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Поддерживаемые модули памяти</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Разъем PS/2</t>
+          <t>64 ГБ</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Кол-во внешних USB 2.0</t>
+          <t>двухканальный</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Режим работы оперативной памяти</t>
+          <t>4</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Слотов PCI-E x1</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Сетевой интерфейс</t>
+          <t>2</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>Разъемов D-Sub (VGA)</t>
+          <t>8 каналов (7.1)</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>Кол-во внешних USB 3.0</t>
+          <t>mATX</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>Сетевой контроллер</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>Звук</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>Аудио контроллер</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>Форм-фактор</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>Питание материнской платы и процессора</t>
-        </is>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>Тип поставки</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>Габариты упаковки (ед) ДхШхВ</t>
-        </is>
-      </c>
-      <c r="V2" t="inlineStr">
-        <is>
-          <t>Вес упаковки (ед)</t>
-        </is>
-      </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>Гарантия</t>
+          <t>24+8 pin</t>
         </is>
       </c>
     </row>
@@ -3659,99 +3339,64 @@
           <t>LGA 1200</t>
         </is>
       </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Intel H470</t>
+        </is>
+      </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Частотная спецификация памяти</t>
+          <t>DIMM</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2933 МГц</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Разъем PS/2</t>
+          <t>64 ГБ</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Разъемов D-Sub (VGA)</t>
+          <t>двухканальный</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Режим работы оперативной памяти</t>
+          <t>4</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Слотов PCI-E x1</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Сетевой интерфейс</t>
+          <t>2</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>Кол-во внешних USB 3.0</t>
+          <t>8 каналов (7.1)</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>mATX</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Звук</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>Аудио контроллер</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>Питание материнской платы и процессора</t>
-        </is>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>Тип поставки</t>
-        </is>
-      </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>Вес упаковки (ед)</t>
-        </is>
-      </c>
-      <c r="X3" t="inlineStr">
-        <is>
-          <t>Тип поддерживаемой памяти</t>
-        </is>
-      </c>
-      <c r="Y3" t="inlineStr">
-        <is>
-          <t>Поддержка частот оперативной памяти</t>
-        </is>
-      </c>
-      <c r="Z3" t="inlineStr">
-        <is>
-          <t>Поддерживаемые модули памяти</t>
-        </is>
-      </c>
-      <c r="AA3" t="inlineStr">
-        <is>
-          <t>Разъемов SATA3</t>
-        </is>
-      </c>
-      <c r="AB3" t="inlineStr">
-        <is>
-          <t>Кол-во внешних USB 2.0</t>
-        </is>
-      </c>
-      <c r="AC3" t="inlineStr">
-        <is>
-          <t>Форм-фактор</t>
-        </is>
-      </c>
-      <c r="AD3" t="inlineStr">
-        <is>
-          <t>Гарантия</t>
+          <t>24+8 pin</t>
         </is>
       </c>
     </row>
@@ -3771,109 +3416,64 @@
           <t>SocketAM4</t>
         </is>
       </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>AMD B450</t>
+        </is>
+      </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Частотная спецификация памяти</t>
+          <t>DIMM</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2933 МГц</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Поддержка SATA RAID</t>
+          <t>32 ГБ</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Разъемов D-Sub (VGA)</t>
+          <t>двухканальный</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>4</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Слотов PCI-E x1</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Сетевой интерфейс</t>
+          <t>4</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>Кол-во внешних USB 2.0</t>
+          <t>8 каналов (7.1)</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>mATX</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Сетевой контроллер</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>Аудио контроллер</t>
-        </is>
-      </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>Питание материнской платы и процессора</t>
-        </is>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>Тип поставки</t>
-        </is>
-      </c>
-      <c r="U4" t="inlineStr">
-        <is>
-          <t>Габариты упаковки (ед) ДхШхВ</t>
-        </is>
-      </c>
-      <c r="Y4" t="inlineStr">
-        <is>
-          <t>Поддержка частот оперативной памяти</t>
-        </is>
-      </c>
-      <c r="AA4" t="inlineStr">
-        <is>
-          <t>Разъем PS/2</t>
-        </is>
-      </c>
-      <c r="AB4" t="inlineStr">
-        <is>
-          <t>Кол-во внешних USB 3.0</t>
-        </is>
-      </c>
-      <c r="AC4" t="inlineStr">
-        <is>
-          <t>Звук</t>
-        </is>
-      </c>
-      <c r="AE4" t="inlineStr">
-        <is>
-          <t>Тип поддерживаемой памяти</t>
-        </is>
-      </c>
-      <c r="AF4" t="inlineStr">
-        <is>
-          <t>Поддерживаемые модули памяти</t>
-        </is>
-      </c>
-      <c r="AG4" t="inlineStr">
-        <is>
-          <t>Режим работы оперативной памяти</t>
-        </is>
-      </c>
-      <c r="AH4" t="inlineStr">
-        <is>
-          <t>Форм-фактор</t>
-        </is>
-      </c>
-      <c r="AI4" t="inlineStr">
-        <is>
-          <t>Вес упаковки (ед)</t>
-        </is>
-      </c>
-      <c r="AJ4" t="inlineStr">
-        <is>
-          <t>Гарантия</t>
+          <t>24+8 pin</t>
         </is>
       </c>
     </row>
@@ -3893,114 +3493,64 @@
           <t>SocketAM5</t>
         </is>
       </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>AMD X670</t>
+        </is>
+      </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Частотная спецификация памяти</t>
+          <t>DIMM</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>5200 МГц</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Поддержка SATA RAID</t>
+          <t>128 ГБ</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Кол-во внешних USB 3.2 (Type-C)</t>
+          <t>двухканальный</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>4</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Слотов PCI-E 3.0&amp;nbsp;x16</t>
+          <t>4</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Особенности внешних разъемов</t>
+          <t>6</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>Кол-во внешних USB 3.0</t>
-        </is>
-      </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>Форм-фактор</t>
-        </is>
-      </c>
-      <c r="U5" t="inlineStr">
-        <is>
-          <t>Вес упаковки (ед)</t>
-        </is>
-      </c>
-      <c r="AA5" t="inlineStr">
-        <is>
-          <t>Звук</t>
-        </is>
-      </c>
-      <c r="AC5" t="inlineStr">
-        <is>
-          <t>WiFi в стандартной поставке</t>
-        </is>
-      </c>
-      <c r="AK5" t="inlineStr">
-        <is>
-          <t>Поддержка SLI/CrossFire</t>
-        </is>
-      </c>
-      <c r="AL5" t="inlineStr">
-        <is>
-          <t>Тип поддерживаемой памяти</t>
-        </is>
-      </c>
-      <c r="AM5" t="inlineStr">
-        <is>
-          <t>Поддержка частот оперативной памяти</t>
-        </is>
-      </c>
-      <c r="AN5" t="inlineStr">
-        <is>
-          <t>Поддерживаемые модули памяти</t>
-        </is>
-      </c>
-      <c r="AO5" t="inlineStr">
-        <is>
-          <t>Режим работы оперативной памяти</t>
-        </is>
-      </c>
-      <c r="AP5" t="inlineStr">
-        <is>
-          <t>Разъемов SATA3</t>
-        </is>
-      </c>
-      <c r="AQ5" t="inlineStr">
-        <is>
-          <t>Кол-во внешних USB 3.1</t>
-        </is>
-      </c>
-      <c r="AR5" t="inlineStr">
-        <is>
-          <t>Сетевой интерфейс</t>
-        </is>
-      </c>
-      <c r="AS5" t="inlineStr">
-        <is>
-          <t>Сетевой контроллер</t>
-        </is>
-      </c>
-      <c r="AT5" t="inlineStr">
-        <is>
-          <t>Питание материнской платы и процессора</t>
-        </is>
-      </c>
-      <c r="AU5" t="inlineStr">
-        <is>
-          <t>Тип поставки</t>
-        </is>
-      </c>
-      <c r="AV5" t="inlineStr">
-        <is>
-          <t>Гарантия</t>
+          <t>8 каналов (7.1)</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>ATX</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>24+8+8 pin</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -4020,114 +3570,64 @@
           <t>SocketAM5</t>
         </is>
       </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>AMD X670</t>
+        </is>
+      </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Частотная спецификация памяти</t>
+          <t>DIMM</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>5200 МГц</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Поддержка SATA RAID</t>
+          <t>128 ГБ</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Кол-во внешних USB 3.2 (Type-C)</t>
+          <t>двухканальный</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>4</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Слотов PCI-E 3.0&amp;nbsp;x16</t>
+          <t>4</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Особенности внешних разъемов</t>
+          <t>6</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>Поддерживаемые диски и накопители</t>
-        </is>
-      </c>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t>Форм-фактор</t>
-        </is>
-      </c>
-      <c r="U6" t="inlineStr">
-        <is>
-          <t>Вес упаковки (ед)</t>
-        </is>
-      </c>
-      <c r="AA6" t="inlineStr">
-        <is>
-          <t>Звук</t>
-        </is>
-      </c>
-      <c r="AC6" t="inlineStr">
-        <is>
-          <t>WiFi в стандартной поставке</t>
-        </is>
-      </c>
-      <c r="AK6" t="inlineStr">
-        <is>
-          <t>Поддержка SLI/CrossFire</t>
-        </is>
-      </c>
-      <c r="AL6" t="inlineStr">
-        <is>
-          <t>Тип поддерживаемой памяти</t>
-        </is>
-      </c>
-      <c r="AM6" t="inlineStr">
-        <is>
-          <t>Поддержка частот оперативной памяти</t>
-        </is>
-      </c>
-      <c r="AO6" t="inlineStr">
-        <is>
-          <t>Режим работы оперативной памяти</t>
-        </is>
-      </c>
-      <c r="AP6" t="inlineStr">
-        <is>
-          <t>Разъемов SATA3</t>
-        </is>
-      </c>
-      <c r="AQ6" t="inlineStr">
-        <is>
-          <t>Кол-во внешних USB 3.1</t>
-        </is>
-      </c>
-      <c r="AR6" t="inlineStr">
-        <is>
-          <t>Сетевой интерфейс</t>
-        </is>
-      </c>
-      <c r="AS6" t="inlineStr">
-        <is>
-          <t>Сетевой контроллер</t>
-        </is>
-      </c>
-      <c r="AT6" t="inlineStr">
-        <is>
-          <t>Питание материнской платы и процессора</t>
-        </is>
-      </c>
-      <c r="AU6" t="inlineStr">
-        <is>
-          <t>Тип поставки</t>
-        </is>
-      </c>
-      <c r="AW6" t="inlineStr">
-        <is>
-          <t>Поддерживаемые модули памяти</t>
-        </is>
-      </c>
-      <c r="AX6" t="inlineStr">
-        <is>
-          <t>Гарантия</t>
+          <t>8 каналов (7.1)</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>ATX</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>24+8+8 pin</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>4</t>
         </is>
       </c>
     </row>

</xml_diff>